<commit_message>
Adding Module 1 & 2.
</commit_message>
<xml_diff>
--- a/NPM_SDPP_Task_C5.xlsx
+++ b/NPM_SDPP_Task_C5.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IBCS-PrimaX\Work\Planning IDSDP\Documentation\New folder\SDPP-SRS-BR-FR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Planning Commission\Component 5 doc\git\SDPP-SRS-BR-FR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42C25DC-15B7-4E93-8C3A-E80E919C4531}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component " sheetId="1" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="427">
   <si>
     <t>SL</t>
   </si>
@@ -1190,15 +1191,238 @@
   <si>
     <t>The notifications will use different medium according to BR-C5-M6.</t>
   </si>
+  <si>
+    <t>BR-C5-M1-00001</t>
+  </si>
+  <si>
+    <t>Content management</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00001-FR-00001</t>
+  </si>
+  <si>
+    <t>Can create new content with component and module wise from drop down including file upload.</t>
+  </si>
+  <si>
+    <t>Super Admin, 
+Admin, Component wise users</t>
+  </si>
+  <si>
+    <t>MOC-C5-M1-00001</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00001-FR-00002</t>
+  </si>
+  <si>
+    <t>Can view list of Contents with title, component, module, file, content, link and action column and value.</t>
+  </si>
+  <si>
+    <t>MOC-C5-M1-00002</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00001-FR-00003</t>
+  </si>
+  <si>
+    <t>View individual Content details from list of contents.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00001-FR-00004</t>
+  </si>
+  <si>
+    <t>Can Update Content detail all fields.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00001-FR-00005</t>
+  </si>
+  <si>
+    <t>Delete Content</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00002</t>
+  </si>
+  <si>
+    <t>Smart Search</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00002-FR-00001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin can do only component wise search. </t>
+  </si>
+  <si>
+    <t>MOC-C5-M1-00003</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00002-FR-00002</t>
+  </si>
+  <si>
+    <t>Can search by text with selected component or without selected component.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00002-FR-00003</t>
+  </si>
+  <si>
+    <t>Autocomplete text or suggestions appear
+while admin write any text in search text 
+field.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00002-FR-00004</t>
+  </si>
+  <si>
+    <t>Admin can view the search result as a list
+where three columns will be available 
+Component name, Result and file with all
+type of file that is included with search name in component.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00002-FR-00005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin can download any type of file (Docx, PPT, PDF etc.) by clicking the file type icon from the search result file column. </t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00003</t>
+  </si>
+  <si>
+    <t>Dynamic FAQ Management</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00003-FR-00001</t>
+  </si>
+  <si>
+    <t>Admin can add component and module wise question and answer.</t>
+  </si>
+  <si>
+    <t>MOC-C5-M1-00004</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00003-FR-00002</t>
+  </si>
+  <si>
+    <t>Admin can view List of FAQ in table with edit and delete tab.</t>
+  </si>
+  <si>
+    <t>MOC-C5-M1-00005</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00003-FR-00003</t>
+  </si>
+  <si>
+    <t>Admin can view individual FAQ by selecting FAQ from list of FAQ table.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00003-FR-00004</t>
+  </si>
+  <si>
+    <t>Can edit individual FAQ from clicking edit button in list of FAQ table.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00003-FR-00005</t>
+  </si>
+  <si>
+    <t>Can delete individual FAQ from clicking delete button in list of FAQ table.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00004</t>
+  </si>
+  <si>
+    <t>Live Chat</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00004-FR-00001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Admin can add predefined question and answer for end user for initial chatting before assigning any system user. 
+</t>
+  </si>
+  <si>
+    <t>MOC-C5-M1-00006</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00004-FR-00002</t>
+  </si>
+  <si>
+    <t>System Admin can edit predefined question 
+and answer.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00004-FR-00003</t>
+  </si>
+  <si>
+    <t>System Admin can Delete individual 
+predefined question and answer.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00004-FR-00004</t>
+  </si>
+  <si>
+    <t>System Amin can view list of predefined question and answer for end user in a list table.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00004-FR-00005</t>
+  </si>
+  <si>
+    <t>Real time notification came when any end user wants to chat with system user.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00004-FR-00006</t>
+  </si>
+  <si>
+    <t>System admin can assign system user to end user.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00004-FR-00007</t>
+  </si>
+  <si>
+    <t>System Admin can set a predefined message for end user for starting a new chat with system.</t>
+  </si>
+  <si>
+    <t>BR-C5-M1-00004-FR-00008</t>
+  </si>
+  <si>
+    <t>System Admin can view list of chat count for individual system admin in date wise.</t>
+  </si>
+  <si>
+    <t>BR-C5-M2-00001</t>
+  </si>
+  <si>
+    <t>Create and update organogram</t>
+  </si>
+  <si>
+    <t>System Admin can create organogram after
+selecting create new from organogram 
+management where ministry/division, 
+agency, designation and status field are
+available. Status field have only two value
+in dropdown list full time and contractual.
+Ministry/Division and Agency data list 
+comes from e-nothi.</t>
+  </si>
+  <si>
+    <t>Super Admin</t>
+  </si>
+  <si>
+    <t>BR-C5-M2-00001-FR-00002</t>
+  </si>
+  <si>
+    <t>System admin can view the organogram list by default system created organogram value will show in list table with SL, Designation, Ministry/Division, Agency, Status and Action columns. From Action tab admin can edit and delete the system created organogram data. System admin also can select “Collect from Source” radio button where dropdown value will e-Nothi, Doptor, A2i etc. and get button. After selecting one from collect from source list and press the get button admin can view the data in list table also save the data in database table. In organogram management page admin can select default or collect from source radio button for view the as per selecting data in list table.</t>
+  </si>
+  <si>
+    <t>MOC-C5-M2-00007</t>
+  </si>
+  <si>
+    <t>MOC-C5-M2-00008</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1251,6 +1475,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1279,11 +1510,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1371,26 +1602,91 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1427,12 +1723,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1454,64 +1744,117 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="2" builtinId="21"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="0"/>
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1786,7 +2129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1865,10 +2208,10 @@
       <c r="B4" s="5">
         <v>44199</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="19"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
         <v>62</v>
@@ -1882,10 +2225,10 @@
       <c r="B5" s="5">
         <v>44200</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>61</v>
@@ -1899,19 +2242,19 @@
       <c r="B6" s="5">
         <v>44201</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="21" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="24" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1922,15 +2265,15 @@
       <c r="B7" s="5">
         <v>44202</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="24"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="24"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1939,15 +2282,15 @@
       <c r="B8" s="5">
         <v>44203</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="23"/>
       <c r="F8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="24"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1986,7 +2329,7 @@
       <c r="B11" s="5">
         <v>44206</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -2003,7 +2346,7 @@
       <c r="B12" s="5">
         <v>44207</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="2" t="s">
         <v>46</v>
       </c>
@@ -2020,7 +2363,7 @@
       <c r="B13" s="5">
         <v>44208</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="2" t="s">
         <v>46</v>
       </c>
@@ -2035,7 +2378,7 @@
       <c r="B14" s="5">
         <v>44209</v>
       </c>
-      <c r="C14" s="21"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="2" t="s">
         <v>46</v>
       </c>
@@ -2050,7 +2393,7 @@
       <c r="B15" s="5">
         <v>44210</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="2" t="s">
         <v>46</v>
       </c>
@@ -2095,7 +2438,7 @@
       <c r="B18" s="5">
         <v>44213</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="18" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -2112,7 +2455,7 @@
       <c r="B19" s="5">
         <v>44214</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="2" t="s">
         <v>47</v>
       </c>
@@ -2127,7 +2470,7 @@
       <c r="B20" s="5">
         <v>44215</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="2" t="s">
         <v>47</v>
       </c>
@@ -2142,7 +2485,7 @@
       <c r="B21" s="5">
         <v>44216</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="18" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -2159,7 +2502,7 @@
       <c r="B22" s="5">
         <v>44217</v>
       </c>
-      <c r="C22" s="22"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="2" t="s">
         <v>47</v>
       </c>
@@ -2204,7 +2547,7 @@
       <c r="B25" s="5">
         <v>44220</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="18" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -2221,7 +2564,7 @@
       <c r="B26" s="5">
         <v>44221</v>
       </c>
-      <c r="C26" s="21"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="2" t="s">
         <v>48</v>
       </c>
@@ -2236,7 +2579,7 @@
       <c r="B27" s="5">
         <v>44222</v>
       </c>
-      <c r="C27" s="21"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="2" t="s">
         <v>48</v>
       </c>
@@ -2251,7 +2594,7 @@
       <c r="B28" s="5">
         <v>44223</v>
       </c>
-      <c r="C28" s="21"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="2" t="s">
         <v>60</v>
       </c>
@@ -2266,7 +2609,7 @@
       <c r="B29" s="5">
         <v>44224</v>
       </c>
-      <c r="C29" s="22"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="2" t="s">
         <v>60</v>
       </c>
@@ -2337,16 +2680,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C9:D9"/>
@@ -2356,9 +2689,19 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="C11:C15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C25:C29"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G6:G8" location="Integration!A1" display="Integration Sheet"/>
+    <hyperlink ref="G6:G8" location="Integration!A1" display="Integration Sheet" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2366,7 +2709,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2410,7 +2753,7 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>51</v>
       </c>
       <c r="D2" t="s">
@@ -2423,7 +2766,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="24"/>
+      <c r="C3" s="22"/>
       <c r="D3" t="s">
         <v>53</v>
       </c>
@@ -2434,7 +2777,7 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="24"/>
+      <c r="C4" s="22"/>
       <c r="D4" t="s">
         <v>54</v>
       </c>
@@ -2445,7 +2788,7 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="24"/>
+      <c r="C5" s="22"/>
       <c r="D5" t="s">
         <v>55</v>
       </c>
@@ -2456,7 +2799,7 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="25"/>
+      <c r="C6" s="23"/>
       <c r="D6" t="s">
         <v>56</v>
       </c>
@@ -2478,11 +2821,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L96"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120:B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4096,39 +4439,506 @@
       </c>
       <c r="K96" s="42"/>
     </row>
+    <row r="97" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97" s="44" t="s">
+        <v>358</v>
+      </c>
+      <c r="B97" s="44" t="s">
+        <v>359</v>
+      </c>
+      <c r="C97" s="45" t="s">
+        <v>360</v>
+      </c>
+      <c r="D97" s="46" t="s">
+        <v>361</v>
+      </c>
+      <c r="E97" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F97" s="48"/>
+      <c r="G97" s="48"/>
+      <c r="I97" s="50"/>
+      <c r="K97" s="49" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98" s="44"/>
+      <c r="B98" s="44"/>
+      <c r="C98" s="45" t="s">
+        <v>364</v>
+      </c>
+      <c r="D98" s="46" t="s">
+        <v>365</v>
+      </c>
+      <c r="E98" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F98" s="50"/>
+      <c r="G98" s="50"/>
+      <c r="I98" s="50"/>
+      <c r="K98" s="57" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A99" s="44"/>
+      <c r="B99" s="44"/>
+      <c r="C99" s="45" t="s">
+        <v>367</v>
+      </c>
+      <c r="D99" s="46" t="s">
+        <v>368</v>
+      </c>
+      <c r="E99" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F99" s="47"/>
+      <c r="G99" s="47"/>
+      <c r="I99" s="50"/>
+      <c r="K99" s="58"/>
+    </row>
+    <row r="100" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A100" s="44"/>
+      <c r="B100" s="44"/>
+      <c r="C100" s="45" t="s">
+        <v>369</v>
+      </c>
+      <c r="D100" s="46" t="s">
+        <v>370</v>
+      </c>
+      <c r="E100" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F100" s="47"/>
+      <c r="G100" s="47"/>
+      <c r="I100" s="50"/>
+      <c r="K100" s="58"/>
+    </row>
+    <row r="101" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A101" s="44"/>
+      <c r="B101" s="44"/>
+      <c r="C101" s="45" t="s">
+        <v>371</v>
+      </c>
+      <c r="D101" s="46" t="s">
+        <v>372</v>
+      </c>
+      <c r="E101" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F101" s="47"/>
+      <c r="G101" s="47"/>
+      <c r="I101" s="50"/>
+      <c r="K101" s="59"/>
+    </row>
+    <row r="102" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="44" t="s">
+        <v>373</v>
+      </c>
+      <c r="B102" s="51" t="s">
+        <v>374</v>
+      </c>
+      <c r="C102" s="45" t="s">
+        <v>375</v>
+      </c>
+      <c r="D102" s="52" t="s">
+        <v>376</v>
+      </c>
+      <c r="E102" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F102" s="47"/>
+      <c r="G102" s="47"/>
+      <c r="I102" s="50"/>
+      <c r="K102" s="57" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A103" s="44"/>
+      <c r="B103" s="51"/>
+      <c r="C103" s="45" t="s">
+        <v>378</v>
+      </c>
+      <c r="D103" s="46" t="s">
+        <v>379</v>
+      </c>
+      <c r="E103" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F103" s="47"/>
+      <c r="G103" s="47"/>
+      <c r="I103" s="50"/>
+      <c r="K103" s="58"/>
+    </row>
+    <row r="104" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A104" s="44"/>
+      <c r="B104" s="51"/>
+      <c r="C104" s="45" t="s">
+        <v>380</v>
+      </c>
+      <c r="D104" s="46" t="s">
+        <v>381</v>
+      </c>
+      <c r="E104" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F104" s="47"/>
+      <c r="G104" s="47"/>
+      <c r="I104" s="50"/>
+      <c r="K104" s="58"/>
+    </row>
+    <row r="105" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A105" s="44"/>
+      <c r="B105" s="51"/>
+      <c r="C105" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="D105" s="46" t="s">
+        <v>383</v>
+      </c>
+      <c r="E105" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F105" s="47"/>
+      <c r="G105" s="47"/>
+      <c r="I105" s="50"/>
+      <c r="K105" s="58"/>
+    </row>
+    <row r="106" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="44"/>
+      <c r="B106" s="51"/>
+      <c r="C106" s="45" t="s">
+        <v>384</v>
+      </c>
+      <c r="D106" s="46" t="s">
+        <v>385</v>
+      </c>
+      <c r="E106" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F106" s="47"/>
+      <c r="G106" s="47"/>
+      <c r="I106" s="50"/>
+      <c r="K106" s="59"/>
+    </row>
+    <row r="107" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A107" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="B107" s="51" t="s">
+        <v>387</v>
+      </c>
+      <c r="C107" s="45" t="s">
+        <v>388</v>
+      </c>
+      <c r="D107" s="53" t="s">
+        <v>389</v>
+      </c>
+      <c r="E107" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F107" s="47"/>
+      <c r="G107" s="47"/>
+      <c r="I107" s="50"/>
+      <c r="K107" s="49" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108" s="44"/>
+      <c r="B108" s="51"/>
+      <c r="C108" s="45" t="s">
+        <v>391</v>
+      </c>
+      <c r="D108" s="53" t="s">
+        <v>392</v>
+      </c>
+      <c r="E108" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F108" s="49"/>
+      <c r="G108" s="49"/>
+      <c r="I108" s="50"/>
+      <c r="K108" s="57" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A109" s="44"/>
+      <c r="B109" s="51"/>
+      <c r="C109" s="45" t="s">
+        <v>394</v>
+      </c>
+      <c r="D109" s="53" t="s">
+        <v>395</v>
+      </c>
+      <c r="E109" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F109" s="49"/>
+      <c r="G109" s="49"/>
+      <c r="I109" s="50"/>
+      <c r="K109" s="58"/>
+    </row>
+    <row r="110" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110" s="44"/>
+      <c r="B110" s="51"/>
+      <c r="C110" s="45" t="s">
+        <v>396</v>
+      </c>
+      <c r="D110" s="53" t="s">
+        <v>397</v>
+      </c>
+      <c r="E110" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F110" s="50"/>
+      <c r="G110" s="50"/>
+      <c r="I110" s="50"/>
+      <c r="K110" s="58"/>
+    </row>
+    <row r="111" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="44"/>
+      <c r="B111" s="51"/>
+      <c r="C111" s="45" t="s">
+        <v>398</v>
+      </c>
+      <c r="D111" s="53" t="s">
+        <v>399</v>
+      </c>
+      <c r="E111" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F111" s="50"/>
+      <c r="G111" s="50"/>
+      <c r="I111" s="50"/>
+      <c r="K111" s="59"/>
+    </row>
+    <row r="112" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A112" s="44" t="s">
+        <v>400</v>
+      </c>
+      <c r="B112" s="51" t="s">
+        <v>401</v>
+      </c>
+      <c r="C112" s="45" t="s">
+        <v>402</v>
+      </c>
+      <c r="D112" s="53" t="s">
+        <v>403</v>
+      </c>
+      <c r="E112" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F112" s="50"/>
+      <c r="G112" s="50"/>
+      <c r="I112" s="50"/>
+      <c r="K112" s="57" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A113" s="44"/>
+      <c r="B113" s="51"/>
+      <c r="C113" s="45" t="s">
+        <v>405</v>
+      </c>
+      <c r="D113" s="53" t="s">
+        <v>406</v>
+      </c>
+      <c r="E113" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F113" s="47"/>
+      <c r="G113" s="47"/>
+      <c r="H113" s="50"/>
+      <c r="I113" s="50"/>
+      <c r="K113" s="58"/>
+    </row>
+    <row r="114" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A114" s="44"/>
+      <c r="B114" s="51"/>
+      <c r="C114" s="45" t="s">
+        <v>407</v>
+      </c>
+      <c r="D114" s="53" t="s">
+        <v>408</v>
+      </c>
+      <c r="E114" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F114" s="47"/>
+      <c r="G114" s="47"/>
+      <c r="H114" s="50"/>
+      <c r="I114" s="50"/>
+      <c r="K114" s="58"/>
+    </row>
+    <row r="115" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A115" s="44"/>
+      <c r="B115" s="51"/>
+      <c r="C115" s="45" t="s">
+        <v>409</v>
+      </c>
+      <c r="D115" s="53" t="s">
+        <v>410</v>
+      </c>
+      <c r="E115" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F115" s="50"/>
+      <c r="G115" s="50"/>
+      <c r="H115" s="50"/>
+      <c r="I115" s="50"/>
+      <c r="K115" s="58"/>
+    </row>
+    <row r="116" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A116" s="44"/>
+      <c r="B116" s="51"/>
+      <c r="C116" s="45" t="s">
+        <v>411</v>
+      </c>
+      <c r="D116" s="53" t="s">
+        <v>412</v>
+      </c>
+      <c r="E116" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F116" s="47"/>
+      <c r="G116" s="47"/>
+      <c r="H116" s="50"/>
+      <c r="I116" s="50"/>
+      <c r="K116" s="58"/>
+    </row>
+    <row r="117" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A117" s="44"/>
+      <c r="B117" s="51"/>
+      <c r="C117" s="45" t="s">
+        <v>413</v>
+      </c>
+      <c r="D117" s="53" t="s">
+        <v>414</v>
+      </c>
+      <c r="E117" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F117" s="47"/>
+      <c r="G117" s="47"/>
+      <c r="H117" s="50"/>
+      <c r="I117" s="50"/>
+      <c r="K117" s="58"/>
+    </row>
+    <row r="118" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A118" s="44"/>
+      <c r="B118" s="51"/>
+      <c r="C118" s="45" t="s">
+        <v>415</v>
+      </c>
+      <c r="D118" s="53" t="s">
+        <v>416</v>
+      </c>
+      <c r="E118" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F118" s="47"/>
+      <c r="G118" s="47"/>
+      <c r="H118" s="50"/>
+      <c r="I118" s="50"/>
+      <c r="K118" s="58"/>
+    </row>
+    <row r="119" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119" s="44"/>
+      <c r="B119" s="51"/>
+      <c r="C119" s="45" t="s">
+        <v>417</v>
+      </c>
+      <c r="D119" s="53" t="s">
+        <v>418</v>
+      </c>
+      <c r="E119" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F119" s="50"/>
+      <c r="G119" s="50"/>
+      <c r="H119" s="50"/>
+      <c r="I119" s="50"/>
+      <c r="K119" s="59"/>
+    </row>
+    <row r="120" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A120" s="60" t="s">
+        <v>419</v>
+      </c>
+      <c r="B120" s="51" t="s">
+        <v>420</v>
+      </c>
+      <c r="C120" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="D120" s="53" t="s">
+        <v>421</v>
+      </c>
+      <c r="E120" s="49" t="s">
+        <v>422</v>
+      </c>
+      <c r="F120" s="50"/>
+      <c r="G120" s="55"/>
+      <c r="H120" s="56"/>
+      <c r="I120" s="50"/>
+      <c r="K120" s="27" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+      <c r="A121" s="60"/>
+      <c r="B121" s="51"/>
+      <c r="C121" s="45" t="s">
+        <v>423</v>
+      </c>
+      <c r="D121" s="53" t="s">
+        <v>424</v>
+      </c>
+      <c r="E121" s="49" t="s">
+        <v>422</v>
+      </c>
+      <c r="F121" s="50"/>
+      <c r="G121" s="50"/>
+      <c r="H121" s="54"/>
+      <c r="I121" s="50"/>
+      <c r="K121" s="27" t="s">
+        <v>426</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="K92:K94"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="K95:K96"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="K81:K83"/>
-    <mergeCell ref="A84:A91"/>
-    <mergeCell ref="B84:B91"/>
-    <mergeCell ref="K84:K91"/>
-    <mergeCell ref="A69:A76"/>
-    <mergeCell ref="B69:B76"/>
-    <mergeCell ref="K69:K76"/>
-    <mergeCell ref="F72:F74"/>
-    <mergeCell ref="A77:A80"/>
-    <mergeCell ref="B77:B80"/>
-    <mergeCell ref="K77:K80"/>
-    <mergeCell ref="A61:A66"/>
-    <mergeCell ref="B61:B66"/>
-    <mergeCell ref="K61:K66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="K67:K68"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="K12:K16"/>
-    <mergeCell ref="K26:K28"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K7:K8"/>
+  <mergeCells count="75">
+    <mergeCell ref="A112:A119"/>
+    <mergeCell ref="B112:B119"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="K98:K101"/>
+    <mergeCell ref="K102:K106"/>
+    <mergeCell ref="K108:K111"/>
+    <mergeCell ref="K112:K119"/>
+    <mergeCell ref="A97:A101"/>
+    <mergeCell ref="B97:B101"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="B102:B106"/>
+    <mergeCell ref="A107:A111"/>
+    <mergeCell ref="B107:B111"/>
+    <mergeCell ref="A45:A51"/>
+    <mergeCell ref="B45:B51"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="K37:K40"/>
+    <mergeCell ref="K41:K43"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B37:B40"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A9:A10"/>
@@ -4145,20 +4955,37 @@
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="B29:B30"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A45:A51"/>
-    <mergeCell ref="B45:B51"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="K37:K40"/>
-    <mergeCell ref="K41:K43"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="K12:K16"/>
+    <mergeCell ref="K26:K28"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="A61:A66"/>
+    <mergeCell ref="B61:B66"/>
+    <mergeCell ref="K61:K66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="K67:K68"/>
+    <mergeCell ref="A69:A76"/>
+    <mergeCell ref="B69:B76"/>
+    <mergeCell ref="K69:K76"/>
+    <mergeCell ref="F72:F74"/>
+    <mergeCell ref="A77:A80"/>
+    <mergeCell ref="B77:B80"/>
+    <mergeCell ref="K77:K80"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="K81:K83"/>
+    <mergeCell ref="A84:A91"/>
+    <mergeCell ref="B84:B91"/>
+    <mergeCell ref="K84:K91"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="K92:K94"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="K95:K96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4166,7 +4993,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4550,7 +5377,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4674,7 +5501,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4824,7 +5651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5067,7 +5894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>